<commit_message>
Added parts for pre-amp boards
Added parts for pre-amp boards
</commit_message>
<xml_diff>
--- a/electronics_partlist.xlsx
+++ b/electronics_partlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="33600" windowHeight="19180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="195">
   <si>
     <t>Part</t>
   </si>
@@ -93,18 +93,6 @@
     <t>A34442-ND</t>
   </si>
   <si>
-    <t>http://search.digikey.com/us/en/products/DCMA37SA101/IDCMA37SA101-ND/2583993</t>
-  </si>
-  <si>
-    <t>IDCMA37SA101-ND</t>
-  </si>
-  <si>
-    <t>http://search.digikey.com/us/en/products/DCMAY37SA101/IDCMAY37SA101-ND/2584178</t>
-  </si>
-  <si>
-    <t>IDCMAY37SA101-ND</t>
-  </si>
-  <si>
     <t>Retention Clips for D-connectors (4-40)</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>http://www.digikey.com/product-detail/en/GCHDLP62M62M/GCHDLP62M62M-ND/1754471</t>
   </si>
   <si>
-    <t>GCHDLP62M62M-ND</t>
-  </si>
-  <si>
     <t>Gender Changer 62-62 male-male</t>
   </si>
   <si>
@@ -492,9 +477,6 @@
     <t>Circular Connector - 41pin (nonflight)</t>
   </si>
   <si>
-    <t>SMD Components</t>
-  </si>
-  <si>
     <t>Misc</t>
   </si>
   <si>
@@ -520,6 +502,108 @@
   </si>
   <si>
     <t>Yellow Chromate Zinc</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Might have weird insert things in holes.</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DDU50S/IDDU50S-ND/2583240</t>
+  </si>
+  <si>
+    <t>DDU50S</t>
+  </si>
+  <si>
+    <t>too expensive ($100 per)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DDMA50PA191/IDDMA50PA191-ND/2583244</t>
+  </si>
+  <si>
+    <t>DDMA50PA191</t>
+  </si>
+  <si>
+    <t>Potting boot</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DB50906-1/1003-1900-ND/2580740</t>
+  </si>
+  <si>
+    <t>DB50906-1</t>
+  </si>
+  <si>
+    <t>potting boot</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DC50907-1/1003-1901-ND/2580802</t>
+  </si>
+  <si>
+    <t>15 HD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DA50905-1/1003-2007-ND/2580651</t>
+  </si>
+  <si>
+    <t>DA50905-1</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DAMA15SA183/IDAMA15SA183-ND/2582121</t>
+  </si>
+  <si>
+    <t>15 pin D-sub</t>
+  </si>
+  <si>
+    <t>DAMA15SA183</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DAMA15PA152/IDAMA15PA152-ND/2582334</t>
+  </si>
+  <si>
+    <t>DAMA15PA152</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/M24308%2F2-350/IM24308%2F2-350-ND/2494076</t>
+  </si>
+  <si>
+    <t>M24308/2-350</t>
+  </si>
+  <si>
+    <t>a bit cheaper</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DCU37P/IDCU37P-ND/2582599</t>
+  </si>
+  <si>
+    <t>DCU37P</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/M24308%2F2-345F/IM24308%2F2-345F-ND/2489060</t>
+  </si>
+  <si>
+    <t>M24308/2-345F</t>
+  </si>
+  <si>
+    <t>SMD Components for pre-amp board</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/AD620ARZ/AD620ARZ-ND/617755</t>
+  </si>
+  <si>
+    <t>AD620ARZ-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MAX6008AEUR%2BT/MAX6008AEUR%2BTDKR-ND/1987237</t>
+  </si>
+  <si>
+    <t>MAX6008AEUR+TDKR-ND</t>
+  </si>
+  <si>
+    <t>http://www.newadvg.com/</t>
+  </si>
+  <si>
+    <t>LSK170C-SOT23</t>
   </si>
 </sst>
 </file>
@@ -609,7 +693,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -656,8 +740,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -674,8 +780,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -720,6 +829,28 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1050,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S88"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1062,802 +1193,971 @@
     <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="87.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>117</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="10">
         <v>9</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="10">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="E11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="E12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E13" t="s">
-        <v>164</v>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="10">
-        <v>25</v>
-      </c>
-      <c r="B17" s="10"/>
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" t="s">
-        <v>131</v>
+        <v>153</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>14</v>
+        <v>159</v>
+      </c>
+      <c r="E18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
+        <v>175</v>
+      </c>
+      <c r="E19" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="D22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="4"/>
+      <c r="A22" s="10">
+        <v>25</v>
+      </c>
+      <c r="B22" s="10"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
       </c>
       <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" t="s">
-        <v>46</v>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="10">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="D27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
         <v>142</v>
       </c>
-      <c r="B27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="10">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C31" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="10">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>149</v>
-      </c>
-      <c r="B35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" s="3" t="s">
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="10">
+    <row r="44" spans="1:6">
+      <c r="A44" s="10">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C38" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="3" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E47" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" t="s">
-        <v>125</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="D40" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="10">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>150</v>
-      </c>
-      <c r="B44" t="s">
-        <v>131</v>
-      </c>
-      <c r="C44" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19">
-      <c r="A50" s="9" t="s">
-        <v>153</v>
+      <c r="F47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
+      <c r="A49" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="D49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:19">
       <c r="A51" s="10">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:19">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>145</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" t="s">
+        <v>119</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E52" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:19">
       <c r="A53" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E53" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>95</v>
-      </c>
-      <c r="R53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S53" t="s">
-        <v>63</v>
+        <v>145</v>
+      </c>
+      <c r="B53" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:19">
       <c r="A54" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E54" t="s">
-        <v>100</v>
-      </c>
-      <c r="F54" s="4"/>
+        <v>145</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F54" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="55" spans="1:19">
       <c r="A55" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="A60" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
+      <c r="A61" s="10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>90</v>
+      </c>
+      <c r="R63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E64" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D66" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E66" t="s">
         <v>109</v>
       </c>
-      <c r="E55" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="A56" t="s">
+      <c r="F66" s="4"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="16">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="D70" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="D72" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="D75" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="D76" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" ht="16">
+      <c r="A78" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="D78" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F78" s="4"/>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="4" customFormat="1">
+      <c r="A82" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="D82" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q82" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="R82" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" s="4" customFormat="1">
+      <c r="A83" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" t="s">
+        <v>45</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D84" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D85" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="A90" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
+      <c r="A91" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
+      <c r="A92" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
+      <c r="A96" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>111</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="E97" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E98" t="s">
         <v>113</v>
       </c>
-      <c r="E56" t="s">
-        <v>114</v>
-      </c>
-      <c r="F56" s="4"/>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="A58" s="10">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="16">
-      <c r="A59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19">
-      <c r="A60" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="4"/>
-      <c r="D60" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19">
-      <c r="A61" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E61" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19">
-      <c r="A62" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" s="4"/>
-      <c r="D62" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E62" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19">
-      <c r="A64" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
-      <c r="A65" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="D65" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
-      <c r="A66" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="D66" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="4"/>
-    </row>
-    <row r="67" spans="1:18">
-      <c r="A67" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="4"/>
-      <c r="E67" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F67" s="4"/>
-    </row>
-    <row r="68" spans="1:18" ht="16">
-      <c r="A68" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B68" s="4"/>
-      <c r="D68" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F68" s="4"/>
-    </row>
-    <row r="71" spans="1:18">
-      <c r="A71" s="9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" s="4" customFormat="1">
-      <c r="A72" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="D72" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q72" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="R72" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" s="4" customFormat="1">
-      <c r="A73" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18">
-      <c r="A74" t="s">
-        <v>50</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D74" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18">
-      <c r="A75" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D75" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18">
-      <c r="A77" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18">
-      <c r="A78" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18">
-      <c r="A79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18">
-      <c r="A80" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B80" s="4"/>
-      <c r="C80" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B81" s="6"/>
-      <c r="C81" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B82" s="6"/>
-      <c r="C82" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" t="s">
-        <v>116</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E87" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" t="s">
-        <v>119</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E88" t="s">
-        <v>118</v>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="D99" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E99" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="D100" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E100" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="D101" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E101" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E59" r:id="rId1"/>
-    <hyperlink ref="E34" r:id="rId2"/>
-    <hyperlink ref="E35" r:id="rId3"/>
-    <hyperlink ref="E43" r:id="rId4"/>
-    <hyperlink ref="E44" r:id="rId5"/>
-    <hyperlink ref="E27" r:id="rId6"/>
-    <hyperlink ref="E19" r:id="rId7"/>
-    <hyperlink ref="E18" r:id="rId8"/>
+    <hyperlink ref="E69" r:id="rId1"/>
+    <hyperlink ref="E41" r:id="rId2"/>
+    <hyperlink ref="E42" r:id="rId3"/>
+    <hyperlink ref="E52" r:id="rId4"/>
+    <hyperlink ref="E53" r:id="rId5"/>
+    <hyperlink ref="E33" r:id="rId6"/>
+    <hyperlink ref="E24" r:id="rId7"/>
+    <hyperlink ref="E23" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>